<commit_message>
slight UI fixes - feedback popup
</commit_message>
<xml_diff>
--- a/backend/data/feedback.xlsx
+++ b/backend/data/feedback.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>Timestamp</t>
   </si>
@@ -49,12 +49,18 @@
     <t>2026-02-13 16:10:20</t>
   </si>
   <si>
+    <t>2026-02-13 19:16:41</t>
+  </si>
+  <si>
     <t>Akash</t>
   </si>
   <si>
     <t>Earliest Availability Date</t>
   </si>
   <si>
+    <t>Ship From Best Location</t>
+  </si>
+  <si>
     <t>Reports &amp; Email</t>
   </si>
   <si>
@@ -64,6 +70,9 @@
     <t>Metric Cards</t>
   </si>
   <si>
+    <t>Advanced Analysis</t>
+  </si>
+  <si>
     <t>TEST</t>
   </si>
   <si>
@@ -77,6 +86,9 @@
   </si>
   <si>
     <t>gygy</t>
+  </si>
+  <si>
+    <t>ghjghgjhg</t>
   </si>
 </sst>
 </file>
@@ -434,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -465,19 +477,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -485,19 +497,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -505,19 +517,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -525,16 +537,16 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -542,16 +554,36 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>